<commit_message>
update report asset kapal
</commit_message>
<xml_diff>
--- a/report/Custom Report - Asset Kapal.xlsx
+++ b/report/Custom Report - Asset Kapal.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DAE82F-59A0-4078-A053-1BCD2A1F2AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KAPAL" sheetId="1" r:id="rId1"/>
@@ -81,18 +82,6 @@
     <t>NILAI PEROLEHAN</t>
   </si>
   <si>
-    <t>LOA</t>
-  </si>
-  <si>
-    <t>BREADTH</t>
-  </si>
-  <si>
-    <t>DEPTH</t>
-  </si>
-  <si>
-    <t>DRAFT MAX</t>
-  </si>
-  <si>
     <t>TAHUN PEMBUATAN</t>
   </si>
   <si>
@@ -111,15 +100,6 @@
     <t>PORT OF REGISTRATION</t>
   </si>
   <si>
-    <t>GT</t>
-  </si>
-  <si>
-    <t>KECEPATAN</t>
-  </si>
-  <si>
-    <t>BOLLARD PULL</t>
-  </si>
-  <si>
     <t>${table:pk.NAMA_ASSET}</t>
   </si>
   <si>
@@ -181,12 +161,33 @@
   </si>
   <si>
     <t>${table:pk.BREADTH}</t>
+  </si>
+  <si>
+    <t>LOA (M)</t>
+  </si>
+  <si>
+    <t>BREADTH (M)</t>
+  </si>
+  <si>
+    <t>DEPTH (M)</t>
+  </si>
+  <si>
+    <t>DRAFT MAX (M)</t>
+  </si>
+  <si>
+    <t>GT (TON)</t>
+  </si>
+  <si>
+    <t>KECEPATAN (KNOT)</t>
+  </si>
+  <si>
+    <t>BOLLARD PULL (TON)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -573,46 +574,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.21875" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.6640625" customWidth="1"/>
-    <col min="24" max="24" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.7109375" customWidth="1"/>
+    <col min="24" max="24" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -626,55 +626,55 @@
         <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="S1" s="4" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>4</v>
@@ -695,7 +695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -703,61 +703,61 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>10</v>

</xml_diff>